<commit_message>
updated release columns & rebuilt models
</commit_message>
<xml_diff>
--- a/dist/rd3_freeze1.xlsx
+++ b/dist/rd3_freeze1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="271">
   <si>
     <t>rd3</t>
   </si>
@@ -138,6 +138,9 @@
     <t>phenopacketsID</t>
   </si>
   <si>
+    <t>patch</t>
+  </si>
+  <si>
     <t>variant</t>
   </si>
   <si>
@@ -171,9 +174,6 @@
     <t>retracted</t>
   </si>
   <si>
-    <t>patch</t>
-  </si>
-  <si>
     <t>patch_comment</t>
   </si>
   <si>
@@ -339,6 +339,12 @@
     <t>Affected status</t>
   </si>
   <si>
+    <t>Phenotype Patch</t>
+  </si>
+  <si>
+    <t>Subject Releases</t>
+  </si>
+  <si>
     <t>Organisation</t>
   </si>
   <si>
@@ -363,72 +369,84 @@
     <t>Retracted Subject</t>
   </si>
   <si>
-    <t>Patch</t>
+    <t>Release Comments</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Country of Origin</t>
+  </si>
+  <si>
+    <t>Consanguinity suspected</t>
+  </si>
+  <si>
+    <t>Release Comment</t>
+  </si>
+  <si>
+    <t>Claimed sex</t>
+  </si>
+  <si>
+    <t>Observed sex</t>
+  </si>
+  <si>
+    <t>Tissue Types</t>
+  </si>
+  <si>
+    <t>Extracted Protocol</t>
+  </si>
+  <si>
+    <t>QC failed</t>
+  </si>
+  <si>
+    <t>Retracted Sample</t>
+  </si>
+  <si>
+    <t>Date available</t>
+  </si>
+  <si>
+    <t>Batch Number</t>
+  </si>
+  <si>
+    <t>Sample Releases</t>
+  </si>
+  <si>
+    <t>Enrichment kit</t>
+  </si>
+  <si>
+    <t>Library Source</t>
+  </si>
+  <si>
+    <t>Sequencing Centre</t>
+  </si>
+  <si>
+    <t>MeanCov</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>Retracted Experiment</t>
+  </si>
+  <si>
+    <t>Experiment Releases</t>
+  </si>
+  <si>
+    <t>EGA Accession Number</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>Checksum</t>
+  </si>
+  <si>
+    <t>File Releases</t>
   </si>
   <si>
     <t>Patch Comment</t>
   </si>
   <si>
-    <t>Date of Birth</t>
-  </si>
-  <si>
-    <t>Country of Origin</t>
-  </si>
-  <si>
-    <t>Consanguinity suspected</t>
-  </si>
-  <si>
-    <t>Claimed sex</t>
-  </si>
-  <si>
-    <t>Observed sex</t>
-  </si>
-  <si>
-    <t>Tissue Types</t>
-  </si>
-  <si>
-    <t>Extracted Protocol</t>
-  </si>
-  <si>
-    <t>QC failed</t>
-  </si>
-  <si>
-    <t>Retracted Sample</t>
-  </si>
-  <si>
-    <t>Date available</t>
-  </si>
-  <si>
-    <t>Batch Number</t>
-  </si>
-  <si>
-    <t>Enrichment kit</t>
-  </si>
-  <si>
-    <t>Library Source</t>
-  </si>
-  <si>
-    <t>Sequencing Centre</t>
-  </si>
-  <si>
-    <t>MeanCov</t>
-  </si>
-  <si>
-    <t>C20</t>
-  </si>
-  <si>
-    <t>Retracted Experiment</t>
-  </si>
-  <si>
-    <t>EGA Accession Number</t>
-  </si>
-  <si>
-    <t>Filename</t>
-  </si>
-  <si>
-    <t>Checksum</t>
-  </si>
-  <si>
     <t>Created</t>
   </si>
   <si>
@@ -468,6 +486,12 @@
     <t>Relevant Phenotype NOT present in subject</t>
   </si>
   <si>
+    <t>name of the most recent phenopackets file (formated as &lt;subjectID&gt;.&lt;date&gt;.json)</t>
+  </si>
+  <si>
+    <t>One or more RD3 releases associated with the subject</t>
+  </si>
+  <si>
     <t>candidate pathogenic variant(s) for this subject</t>
   </si>
   <si>
@@ -495,9 +519,6 @@
     <t>Is the subject retracted or not</t>
   </si>
   <si>
-    <t>Patch to which the subject belongs</t>
-  </si>
-  <si>
     <t>Date of birth (YYYY) (COMMON DATA ELEMENTS 2.1)</t>
   </si>
   <si>
@@ -555,7 +576,7 @@
     <t>Sample batch number</t>
   </si>
   <si>
-    <t>Patch to which the sample belongs</t>
+    <t>One or more RD3 releases associated with the sample</t>
   </si>
   <si>
     <t>Unique identifier (experimentID + patch)</t>
@@ -600,9 +621,6 @@
     <t>Is the experiment retracted or not</t>
   </si>
   <si>
-    <t>Patch to which the labinfo belongs</t>
-  </si>
-  <si>
     <t>hash code to check if file is not corrupted.</t>
   </si>
   <si>
@@ -612,12 +630,18 @@
     <t>link to file(s) produced for this sample</t>
   </si>
   <si>
-    <t>Patch to which the file belongs</t>
+    <t>One or more RD3 releases associated with the file</t>
   </si>
   <si>
     <t>Creation date in RD3 database</t>
   </si>
   <si>
+    <t>Identifier of the corresponding record in the labinfo table</t>
+  </si>
+  <si>
+    <t>path of the file stored in the sandbox environment</t>
+  </si>
+  <si>
     <t>status of job (running, completed, or error)</t>
   </si>
   <si>
@@ -663,6 +687,9 @@
     <t>mref</t>
   </si>
   <si>
+    <t>categorical_mref</t>
+  </si>
+  <si>
     <t>date</t>
   </si>
   <si>
@@ -675,9 +702,6 @@
     <t>categorical</t>
   </si>
   <si>
-    <t>categorical_mref</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -699,6 +723,9 @@
     <t>rd3_phenotype</t>
   </si>
   <si>
+    <t>rd3_patch</t>
+  </si>
+  <si>
     <t>rd3_variantinfo</t>
   </si>
   <si>
@@ -709,9 +736,6 @@
   </si>
   <si>
     <t>rd3_noyesunknown</t>
-  </si>
-  <si>
-    <t>rd3_patch</t>
   </si>
   <si>
     <t>rd3_pathologicalstate</t>
@@ -1162,13 +1186,13 @@
         <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1211,16 +1235,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1322,61 +1346,61 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -1390,34 +1414,34 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="E2" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="F2" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G2" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="H2" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="I2" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J2" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K2" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L2" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M2" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -1431,34 +1455,34 @@
         <v>101</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F3" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G3" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I3" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J3" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K3" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L3" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="M3" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="N3" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -1472,37 +1496,37 @@
         <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="E4" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F4" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G4" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I4" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J4" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K4" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="L4" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M4" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N4" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O4" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -1516,34 +1540,34 @@
         <v>103</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="E5" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F5" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G5" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I5" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J5" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K5" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L5" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M5" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N5" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -1557,34 +1581,34 @@
         <v>104</v>
       </c>
       <c r="D6" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E6" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F6" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G6" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I6" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J6" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K6" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="L6" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M6" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N6" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O6" t="s">
         <v>23</v>
@@ -1601,34 +1625,34 @@
         <v>105</v>
       </c>
       <c r="D7" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E7" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F7" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G7" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I7" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J7" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K7" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="L7" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M7" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N7" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O7" t="s">
         <v>23</v>
@@ -1645,34 +1669,34 @@
         <v>106</v>
       </c>
       <c r="D8" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E8" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F8" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G8" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I8" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J8" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K8" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="L8" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M8" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N8" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -1686,37 +1710,37 @@
         <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E9" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F9" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G9" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I9" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J9" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K9" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="L9" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M9" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N9" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O9" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -1730,37 +1754,37 @@
         <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="E10" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F10" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G10" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I10" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J10" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K10" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="L10" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M10" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N10" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O10" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -1774,37 +1798,37 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E11" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F11" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G11" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I11" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J11" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K11" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="L11" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M11" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N11" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O11" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -1815,37 +1839,37 @@
         <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>107</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="E12" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F12" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G12" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I12" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J12" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K12" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L12" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M12" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N12" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1856,40 +1880,40 @@
         <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
       <c r="D13" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="E13" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F13" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G13" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I13" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J13" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K13" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="L13" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M13" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N13" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O13" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -1900,40 +1924,40 @@
         <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>107</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="E14" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F14" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G14" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I14" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J14" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K14" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="L14" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M14" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N14" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O14" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -1944,40 +1968,40 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>109</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>159</v>
       </c>
       <c r="E15" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F15" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G15" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I15" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J15" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K15" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="L15" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M15" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N15" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O15" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -1991,34 +2015,37 @@
         <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>152</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F16" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G16" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I16" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J16" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K16" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="L16" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M16" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N16" t="s">
-        <v>208</v>
+        <v>216</v>
+      </c>
+      <c r="O16" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -2029,37 +2056,37 @@
         <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="E17" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F17" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G17" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I17" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J17" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K17" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="L17" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M17" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N17" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -2070,37 +2097,37 @@
         <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D18" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E18" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F18" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G18" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I18" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J18" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K18" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="L18" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M18" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N18" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -2111,34 +2138,37 @@
         <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="D19" t="s">
+        <v>162</v>
       </c>
       <c r="E19" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F19" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G19" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I19" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J19" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K19" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="L19" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M19" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N19" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -2149,40 +2179,34 @@
         <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>111</v>
-      </c>
-      <c r="D20" t="s">
-        <v>155</v>
+        <v>112</v>
       </c>
       <c r="E20" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F20" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G20" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I20" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J20" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K20" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="L20" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M20" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N20" t="s">
-        <v>208</v>
-      </c>
-      <c r="P20" t="s">
-        <v>46</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -2193,40 +2217,40 @@
         <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D21" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="E21" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F21" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G21" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I21" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J21" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K21" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="L21" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M21" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N21" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="P21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -2237,43 +2261,40 @@
         <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D22" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="E22" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F22" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G22" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I22" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J22" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K22" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="L22" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M22" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N22" t="s">
-        <v>208</v>
-      </c>
-      <c r="O22" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="P22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -2284,43 +2305,43 @@
         <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="E23" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F23" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G23" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I23" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J23" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K23" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="L23" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M23" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N23" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O23" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>241</v>
+        <v>239</v>
+      </c>
+      <c r="P23" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -2331,40 +2352,43 @@
         <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D24" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="E24" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F24" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G24" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I24" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J24" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K24" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="L24" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M24" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N24" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O24" t="s">
-        <v>231</v>
+        <v>239</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -2375,37 +2399,37 @@
         <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D25" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="E25" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F25" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G25" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I25" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J25" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K25" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L25" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M25" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N25" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -2419,34 +2443,34 @@
         <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="E26" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="F26" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G26" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="I26" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J26" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K26" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L26" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M26" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="R26" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -2460,40 +2484,40 @@
         <v>101</v>
       </c>
       <c r="D27" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="E27" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="F27" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G27" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I27" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J27" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K27" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="L27" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M27" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N27" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O27" t="s">
         <v>23</v>
       </c>
       <c r="R27" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -2504,37 +2528,37 @@
         <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D28" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E28" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F28" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G28" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I28" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J28" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K28" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="L28" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M28" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N28" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -2548,34 +2572,34 @@
         <v>54</v>
       </c>
       <c r="D29" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="E29" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F29" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G29" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I29" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J29" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K29" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="L29" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M29" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N29" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -2589,37 +2613,37 @@
         <v>55</v>
       </c>
       <c r="D30" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="E30" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F30" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G30" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I30" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J30" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K30" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="L30" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M30" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N30" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O30" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -2633,34 +2657,34 @@
         <v>56</v>
       </c>
       <c r="D31" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="E31" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F31" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G31" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I31" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J31" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K31" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="L31" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M31" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N31" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -2671,37 +2695,37 @@
         <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D32" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="E32" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F32" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G32" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I32" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J32" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K32" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L32" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M32" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N32" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -2712,37 +2736,37 @@
         <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D33" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E33" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F33" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G33" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I33" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J33" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K33" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="L33" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M33" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N33" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -2750,43 +2774,43 @@
         <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E34" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F34" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G34" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I34" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J34" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K34" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="L34" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M34" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N34" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O34" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -2797,37 +2821,37 @@
         <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D35" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="E35" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F35" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G35" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I35" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J35" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K35" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L35" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M35" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N35" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -2841,34 +2865,34 @@
         <v>29</v>
       </c>
       <c r="D36" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E36" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="F36" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G36" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="I36" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J36" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K36" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L36" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M36" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="R36" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -2882,37 +2906,37 @@
         <v>59</v>
       </c>
       <c r="D37" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="E37" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F37" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G37" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I37" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J37" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K37" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L37" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="M37" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="N37" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="R37" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -2926,34 +2950,34 @@
         <v>60</v>
       </c>
       <c r="D38" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="E38" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F38" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G38" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I38" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J38" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K38" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L38" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M38" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N38" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -2967,34 +2991,34 @@
         <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E39" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F39" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G39" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I39" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J39" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K39" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="L39" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M39" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N39" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O39" t="s">
         <v>23</v>
@@ -3011,34 +3035,34 @@
         <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="E40" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F40" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G40" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I40" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J40" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K40" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="L40" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M40" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N40" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -3049,40 +3073,40 @@
         <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D41" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="E41" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F41" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G41" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I41" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J41" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K41" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="L41" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M41" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N41" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O41" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
     <row r="42" spans="1:18">
@@ -3093,40 +3117,40 @@
         <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D42" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E42" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F42" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G42" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I42" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J42" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K42" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="L42" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M42" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N42" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O42" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
     <row r="43" spans="1:18">
@@ -3137,37 +3161,37 @@
         <v>63</v>
       </c>
       <c r="D43" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="E43" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F43" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G43" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I43" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J43" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K43" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="L43" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M43" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N43" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O43" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
     </row>
     <row r="44" spans="1:18">
@@ -3178,34 +3202,34 @@
         <v>64</v>
       </c>
       <c r="D44" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="E44" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F44" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G44" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I44" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J44" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K44" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="L44" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M44" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N44" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="45" spans="1:18">
@@ -3216,37 +3240,37 @@
         <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E45" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F45" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G45" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I45" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J45" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K45" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="L45" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M45" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N45" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O45" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
     </row>
     <row r="46" spans="1:18">
@@ -3257,34 +3281,34 @@
         <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E46" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F46" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G46" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I46" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J46" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K46" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L46" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M46" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N46" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="1:18">
@@ -3298,37 +3322,37 @@
         <v>67</v>
       </c>
       <c r="D47" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="E47" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F47" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G47" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I47" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J47" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K47" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="L47" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M47" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N47" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O47" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
     </row>
     <row r="48" spans="1:18">
@@ -3339,37 +3363,37 @@
         <v>68</v>
       </c>
       <c r="C48" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D48" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="E48" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F48" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G48" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I48" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J48" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K48" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="L48" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M48" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N48" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49" spans="1:18">
@@ -3377,43 +3401,43 @@
         <v>25</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C49" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D49" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="E49" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F49" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G49" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I49" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J49" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K49" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="L49" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M49" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N49" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O49" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
     </row>
     <row r="50" spans="1:18">
@@ -3421,43 +3445,43 @@
         <v>25</v>
       </c>
       <c r="B50" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C50" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D50" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E50" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F50" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G50" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I50" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J50" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K50" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="L50" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M50" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N50" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O50" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
     </row>
     <row r="51" spans="1:18">
@@ -3465,43 +3489,43 @@
         <v>25</v>
       </c>
       <c r="B51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C51" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E51" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F51" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G51" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I51" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J51" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K51" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="L51" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M51" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N51" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O51" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="Q51" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="52" spans="1:18">
@@ -3512,37 +3536,37 @@
         <v>69</v>
       </c>
       <c r="C52" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D52" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="E52" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F52" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G52" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I52" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J52" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K52" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="L52" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M52" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N52" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="53" spans="1:18">
@@ -3556,34 +3580,34 @@
         <v>70</v>
       </c>
       <c r="E53" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F53" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G53" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I53" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J53" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K53" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="L53" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M53" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N53" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O53" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
     </row>
     <row r="54" spans="1:18">
@@ -3594,37 +3618,37 @@
         <v>71</v>
       </c>
       <c r="C54" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D54" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E54" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F54" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G54" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I54" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J54" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K54" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L54" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M54" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N54" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="55" spans="1:18">
@@ -3632,43 +3656,43 @@
         <v>25</v>
       </c>
       <c r="B55" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="D55" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="E55" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F55" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G55" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I55" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J55" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K55" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="L55" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M55" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N55" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O55" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="56" spans="1:18">
@@ -3679,37 +3703,37 @@
         <v>52</v>
       </c>
       <c r="C56" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D56" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="E56" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F56" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G56" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I56" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J56" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K56" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L56" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M56" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N56" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="57" spans="1:18">
@@ -3723,34 +3747,34 @@
         <v>29</v>
       </c>
       <c r="D57" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="E57" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="F57" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G57" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="I57" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J57" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K57" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L57" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M57" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="R57" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58" spans="1:18">
@@ -3764,34 +3788,34 @@
         <v>72</v>
       </c>
       <c r="D58" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="E58" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F58" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G58" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I58" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J58" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K58" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L58" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="M58" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="N58" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="59" spans="1:18">
@@ -3805,34 +3829,34 @@
         <v>7</v>
       </c>
       <c r="D59" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="E59" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F59" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G59" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I59" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J59" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K59" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="L59" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M59" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N59" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O59" t="s">
         <v>25</v>
@@ -3846,37 +3870,37 @@
         <v>73</v>
       </c>
       <c r="C60" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D60" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E60" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F60" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G60" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I60" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J60" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K60" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L60" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M60" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N60" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="61" spans="1:18">
@@ -3887,40 +3911,40 @@
         <v>74</v>
       </c>
       <c r="C61" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D61" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="E61" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F61" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G61" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I61" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J61" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K61" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="L61" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M61" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N61" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O61" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
     </row>
     <row r="62" spans="1:18">
@@ -3934,34 +3958,34 @@
         <v>75</v>
       </c>
       <c r="D62" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="E62" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F62" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G62" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I62" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J62" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K62" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L62" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M62" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N62" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="63" spans="1:18">
@@ -3975,34 +3999,34 @@
         <v>76</v>
       </c>
       <c r="D63" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="E63" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F63" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G63" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I63" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J63" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K63" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L63" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M63" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N63" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="64" spans="1:18">
@@ -4016,34 +4040,34 @@
         <v>77</v>
       </c>
       <c r="D64" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="E64" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F64" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G64" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I64" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J64" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K64" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L64" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M64" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N64" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="65" spans="1:18">
@@ -4057,37 +4081,37 @@
         <v>78</v>
       </c>
       <c r="D65" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="E65" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F65" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G65" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I65" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J65" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K65" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="L65" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M65" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N65" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O65" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:18">
@@ -4098,37 +4122,37 @@
         <v>79</v>
       </c>
       <c r="C66" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D66" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="E66" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F66" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G66" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I66" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J66" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K66" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L66" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M66" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N66" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="67" spans="1:18">
@@ -4142,34 +4166,34 @@
         <v>80</v>
       </c>
       <c r="D67" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="E67" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F67" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G67" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I67" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J67" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K67" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L67" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M67" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N67" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="68" spans="1:18">
@@ -4183,37 +4207,37 @@
         <v>81</v>
       </c>
       <c r="D68" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="E68" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F68" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G68" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I68" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J68" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K68" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="L68" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M68" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N68" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O68" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
     </row>
     <row r="69" spans="1:18">
@@ -4230,31 +4254,31 @@
         <v>82</v>
       </c>
       <c r="E69" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F69" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G69" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I69" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J69" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K69" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L69" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M69" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N69" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="70" spans="1:18">
@@ -4265,37 +4289,37 @@
         <v>83</v>
       </c>
       <c r="C70" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D70" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="E70" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F70" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G70" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I70" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J70" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K70" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="L70" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M70" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N70" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="71" spans="1:18">
@@ -4306,37 +4330,37 @@
         <v>84</v>
       </c>
       <c r="C71" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D71" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="E71" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F71" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G71" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I71" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J71" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K71" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="L71" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M71" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N71" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="72" spans="1:18">
@@ -4344,46 +4368,46 @@
         <v>26</v>
       </c>
       <c r="B72" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C72" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D72" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="E72" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F72" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G72" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I72" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J72" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K72" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="L72" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M72" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N72" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O72" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="Q72" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:18">
@@ -4391,43 +4415,43 @@
         <v>26</v>
       </c>
       <c r="B73" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C73" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="D73" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="E73" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F73" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G73" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I73" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J73" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K73" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="L73" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M73" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N73" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O73" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="74" spans="1:18">
@@ -4438,37 +4462,37 @@
         <v>52</v>
       </c>
       <c r="C74" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D74" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="E74" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F74" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G74" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I74" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J74" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K74" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L74" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M74" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N74" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="75" spans="1:18">
@@ -4479,37 +4503,37 @@
         <v>85</v>
       </c>
       <c r="C75" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D75" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E75" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="F75" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G75" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="I75" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J75" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K75" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L75" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="M75" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="R75" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="76" spans="1:18">
@@ -4520,37 +4544,37 @@
         <v>86</v>
       </c>
       <c r="C76" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D76" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E76" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="F76" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G76" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I76" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J76" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K76" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L76" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M76" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="N76" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77" spans="1:18">
@@ -4561,37 +4585,37 @@
         <v>87</v>
       </c>
       <c r="C77" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D77" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="E77" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F77" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G77" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I77" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J77" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K77" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L77" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M77" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N77" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="78" spans="1:18">
@@ -4605,37 +4629,37 @@
         <v>88</v>
       </c>
       <c r="D78" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="E78" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="F78" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G78" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I78" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="J78" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K78" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="L78" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M78" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N78" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O78" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
     </row>
     <row r="79" spans="1:18">
@@ -4649,34 +4673,34 @@
         <v>89</v>
       </c>
       <c r="D79" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="E79" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F79" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G79" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I79" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J79" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K79" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="L79" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M79" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N79" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O79" t="s">
         <v>25</v>
@@ -4693,34 +4717,34 @@
         <v>101</v>
       </c>
       <c r="D80" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="E80" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F80" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G80" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I80" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J80" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K80" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="L80" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M80" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N80" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O80" t="s">
         <v>23</v>
@@ -4731,43 +4755,43 @@
         <v>27</v>
       </c>
       <c r="B81" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C81" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="D81" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="E81" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F81" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G81" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I81" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J81" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K81" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="L81" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M81" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N81" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O81" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="82" spans="1:19">
@@ -4778,37 +4802,37 @@
         <v>52</v>
       </c>
       <c r="C82" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="D82" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="E82" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F82" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G82" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I82" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J82" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K82" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L82" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M82" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N82" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="83" spans="1:19">
@@ -4819,37 +4843,37 @@
         <v>90</v>
       </c>
       <c r="C83" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D83" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="E83" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F83" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G83" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I83" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J83" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K83" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="L83" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M83" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N83" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="84" spans="1:19">
@@ -4860,34 +4884,34 @@
         <v>91</v>
       </c>
       <c r="C84" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="E84" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F84" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G84" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I84" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J84" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K84" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="L84" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M84" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N84" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="85" spans="1:19">
@@ -4900,32 +4924,35 @@
       <c r="C85" t="s">
         <v>72</v>
       </c>
+      <c r="D85" t="s">
+        <v>206</v>
+      </c>
       <c r="E85" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F85" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G85" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I85" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J85" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K85" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L85" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M85" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N85" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="86" spans="1:19">
@@ -4936,37 +4963,37 @@
         <v>92</v>
       </c>
       <c r="C86" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D86" t="s">
-        <v>139</v>
+        <v>207</v>
       </c>
       <c r="E86" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F86" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G86" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I86" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J86" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K86" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L86" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M86" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N86" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="87" spans="1:19">
@@ -4980,37 +5007,37 @@
         <v>93</v>
       </c>
       <c r="D87" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="E87" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F87" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G87" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I87" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J87" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K87" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="L87" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M87" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N87" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="S87" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
     </row>
     <row r="88" spans="1:19">
@@ -5024,34 +5051,34 @@
         <v>94</v>
       </c>
       <c r="D88" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="E88" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="F88" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G88" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="I88" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J88" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K88" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L88" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="M88" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="R88" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="89" spans="1:19">
@@ -5065,37 +5092,37 @@
         <v>95</v>
       </c>
       <c r="D89" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="E89" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="F89" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G89" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I89" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J89" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K89" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="L89" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M89" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N89" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O89" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
     </row>
     <row r="90" spans="1:19">
@@ -5109,34 +5136,34 @@
         <v>96</v>
       </c>
       <c r="D90" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="E90" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F90" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G90" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I90" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J90" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K90" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L90" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M90" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N90" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="91" spans="1:19">
@@ -5150,34 +5177,34 @@
         <v>97</v>
       </c>
       <c r="D91" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="E91" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F91" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G91" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I91" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J91" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K91" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="L91" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M91" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N91" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O91" t="s">
         <v>27</v>
@@ -5194,34 +5221,34 @@
         <v>98</v>
       </c>
       <c r="D92" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="E92" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F92" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G92" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I92" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J92" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K92" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="L92" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M92" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N92" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="O92" t="s">
         <v>27</v>
@@ -5238,34 +5265,34 @@
         <v>99</v>
       </c>
       <c r="D93" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="E93" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F93" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G93" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I93" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J93" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K93" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="L93" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M93" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N93" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="94" spans="1:19">
@@ -5279,34 +5306,34 @@
         <v>100</v>
       </c>
       <c r="D94" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="E94" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F94" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G94" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I94" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J94" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K94" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="L94" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="M94" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="N94" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revised display label and description in files table
</commit_message>
<xml_diff>
--- a/dist/rd3_freeze1.xlsx
+++ b/dist/rd3_freeze1.xlsx
@@ -453,7 +453,7 @@
     <t>Extra Information</t>
   </si>
   <si>
-    <t>Filepath Sandbox</t>
+    <t>Fender Filepath</t>
   </si>
   <si>
     <t>Unique identifier (subjectID + patch number)</t>
@@ -639,7 +639,7 @@
     <t>Identifier of the corresponding record in the labinfo table</t>
   </si>
   <si>
-    <t>path of the file stored in the sandbox environment</t>
+    <t>location of the file on Fender. For Gearshift, recode 'solve-rd' to 'umcg-solve-rd'.</t>
   </si>
   <si>
     <t>status of job (running, completed, or error)</t>
@@ -4984,7 +4984,7 @@
         <v>216</v>
       </c>
       <c r="K86" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="L86" t="s">
         <v>216</v>

</xml_diff>